<commit_message>
Idejau savo week ir pakeiciau total i excelio formule
</commit_message>
<xml_diff>
--- a/WEEK formos/WEEK 04-13.xlsx
+++ b/WEEK formos/WEEK 04-13.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denis\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{5B51389C-A598-4080-AA2E-CB60ECC231A4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{8BE80459-82CB-424F-B802-6F22B3589F5A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Week" sheetId="1" r:id="rId1"/>
@@ -40,9 +34,9 @@
     <definedName name="validTeamMembersInitials">[1]Team!$C$2:$C$21</definedName>
     <definedName name="WEEKData">Week!$G$7:$G$11,Week!$I$7:$I$11,Week!$C$15:$C$20,Week!$E$15:$E$20,Week!$G$15:$G$20,Week!$I$15:$I$20</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -157,11 +151,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -343,63 +337,8 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="15" max="30000" min="1" page="10"/>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>76200</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>19050</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="weekSelector" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
-</file>
-
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Index"/>
@@ -658,7 +597,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -710,7 +649,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -904,22 +843,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFDCE84-FC09-430C-837E-5DB7A69EC70F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="WeekSummary"/>
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12"/>
   <cols>
     <col min="1" max="1" width="30.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="0.85546875" style="2" customWidth="1"/>
@@ -935,7 +874,7 @@
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75">
       <c r="A1" s="24" t="str">
         <f>[0]!TSPProcessName &amp; " Week Summary - Form WEEK"</f>
         <v>TSPi Week Summary - Form WEEK</v>
@@ -945,7 +884,7 @@
       <c r="G1" s="9"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:11" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="16" customFormat="1" ht="12.75">
       <c r="A2" s="22" t="s">
         <v>26</v>
       </c>
@@ -966,7 +905,7 @@
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="1:11" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="16" customFormat="1" ht="12.75">
       <c r="A3" s="22" t="s">
         <v>23</v>
       </c>
@@ -988,7 +927,7 @@
       <c r="J3" s="17"/>
       <c r="K3" s="17"/>
     </row>
-    <row r="4" spans="1:11" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="16" customFormat="1" ht="15.75" customHeight="1">
       <c r="A4" s="22" t="s">
         <v>20</v>
       </c>
@@ -1009,14 +948,14 @@
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="13"/>
       <c r="C5" s="9"/>
       <c r="E5" s="9"/>
       <c r="G5" s="15"/>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="13" t="s">
         <v>18</v>
       </c>
@@ -1029,7 +968,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="10" t="s">
         <v>15</v>
       </c>
@@ -1042,7 +981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
@@ -1055,7 +994,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
@@ -1063,14 +1002,14 @@
       <c r="E9" s="9"/>
       <c r="G9" s="5">
         <f>$G$21</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="I9" s="5">
         <f>$I$21</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="10" t="s">
         <v>12</v>
       </c>
@@ -1078,14 +1017,14 @@
       <c r="E10" s="9"/>
       <c r="G10" s="5">
         <f>$G$9</f>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="I10" s="5">
         <f>$I$9</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="10" t="s">
         <v>11</v>
       </c>
@@ -1098,21 +1037,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="1"/>
       <c r="C12" s="9"/>
       <c r="E12" s="9"/>
       <c r="G12" s="9"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="1"/>
       <c r="C13" s="9"/>
       <c r="E13" s="9"/>
       <c r="G13" s="9"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="24">
       <c r="A14" s="13" t="s">
         <v>10</v>
       </c>
@@ -1129,7 +1068,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" s="10" t="str">
         <f>[1]Roles!A2</f>
         <v>Team Leader</v>
@@ -1139,7 +1078,7 @@
       <c r="G15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="10" t="str">
         <f>[1]Roles!A4</f>
         <v>Development Manager</v>
@@ -1157,7 +1096,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="10" t="str">
         <f>[1]Roles!A6</f>
         <v>Planning Manager</v>
@@ -1175,27 +1114,31 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="10" t="str">
         <f>[1]Roles!A8</f>
         <v>Quality/Process Manager</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="10" t="str">
         <f>[1]Roles!A10</f>
         <v>Support Manager</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C19" s="5">
+        <v>7</v>
+      </c>
+      <c r="E19" s="5">
+        <v>4</v>
+      </c>
+      <c r="G19" s="5">
+        <v>6</v>
+      </c>
+      <c r="I19" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="10">
         <f>[1]Roles!A20</f>
         <v>0</v>
@@ -1205,27 +1148,47 @@
       <c r="G20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="5">
-        <v>8</v>
+        <f>SUM(C15:C20)</f>
+        <v>25</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" ref="D21:I21" si="0">SUM(D15:D20)</f>
+        <v>0</v>
       </c>
       <c r="E21" s="5">
-        <v>5</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="1"/>
       <c r="C22" s="9"/>
       <c r="E22" s="9"/>
       <c r="G22" s="9"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="8" t="s">
         <v>4</v>
       </c>
@@ -1242,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
@@ -1259,7 +1222,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
@@ -1276,7 +1239,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
@@ -1293,7 +1256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
@@ -1310,31 +1273,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="9:9">
       <c r="I33" s="5"/>
     </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="9:9">
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="9:9">
       <c r="I35" s="5"/>
     </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="9:9">
       <c r="I36" s="5"/>
     </row>
   </sheetData>
@@ -1347,35 +1310,6 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L File: &amp;F ! &amp;A&amp;R&amp;D  &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId4" name="weekSelector">
-              <controlPr defaultSize="0" autoPict="0" macro="[0]!WeekSummary.weekSelector_Change">
-                <anchor moveWithCells="1" sizeWithCells="1">
-                  <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>2</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>4</xdr:col>
-                    <xdr:colOff>76200</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
perskirstytos valandos funkcionalumo realizavime
</commit_message>
<xml_diff>
--- a/WEEK formos/WEEK 04-13.xlsx
+++ b/WEEK formos/WEEK 04-13.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaponnik\Desktop\temp\WEEK formos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{257F7A06-FC43-47A8-B5BA-A6BA62F7B4FF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{8BE80459-82CB-424F-B802-6F22B3589F5A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Week" sheetId="1" r:id="rId1"/>
@@ -40,7 +34,7 @@
     <definedName name="validTeamMembersInitials">[1]Team!$C$2:$C$21</definedName>
     <definedName name="WEEKData">Week!$G$7:$G$11,Week!$I$7:$I$11,Week!$C$15:$C$20,Week!$E$15:$E$20,Week!$G$15:$G$20,Week!$I$15:$I$20</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -166,7 +160,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -376,14 +370,11 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
-                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -391,12 +382,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -667,7 +652,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -719,7 +704,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -913,19 +898,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BFDCE84-FC09-430C-837E-5DB7A69EC70F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="WeekSummary"/>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1350,18 +1335,18 @@
         <v>33</v>
       </c>
       <c r="C27" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E27" s="4">
         <v>3</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I27" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
@@ -1369,18 +1354,18 @@
         <v>34</v>
       </c>
       <c r="C28" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E28" s="4">
         <v>2.5</v>
       </c>
       <c r="G28" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I28" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
@@ -1388,18 +1373,18 @@
         <v>32</v>
       </c>
       <c r="C29" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E29" s="4">
         <v>5.5</v>
       </c>
       <c r="G29" s="5">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I29" s="5">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
@@ -1426,18 +1411,18 @@
         <v>31</v>
       </c>
       <c r="C31" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E31" s="4">
         <v>2.5</v>
       </c>
       <c r="G31" s="5">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I31" s="5">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>